<commit_message>
Test common cleaning functions
</commit_message>
<xml_diff>
--- a/CLI_Data_Cleaning_Tool/output.xlsx
+++ b/CLI_Data_Cleaning_Tool/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,142 +425,22 @@
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>john doe</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
-        <is>
-          <t>johndoe@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>john doe</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>johndoe@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>john doe</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>johndoe@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>john doe</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>johndoe@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>john doe</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>johndoe@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>john doe</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>johndoe@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>john doe</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>johndoe@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>john doe</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>johndoe@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>john doe</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>johndoe@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>john doe</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>johndoe@gmail.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>john doe</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
         <is>
           <t>johndoe@gmail.com</t>
         </is>

</xml_diff>